<commit_message>
Aggiunti campi obbligatori per test 448
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111GRUPPOGPI00/ARKO_SRL/cartella_emofilia_rer/1.2/report-checklist.xlsx
+++ b/GATEWAY/A1#111GRUPPOGPI00/ARKO_SRL/cartella_emofilia_rer/1.2/report-checklist.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Sviluppo\github\ministero-salute\it-fse-accreditamento\GATEWAY\A1#111GRUPPOGPI00\ARKO_SRL\cartella_emofilia_rer\1.2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A312FFC-274F-466A-B4E8-B63C309DCD3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{032994A6-DCE4-4A20-81C1-2883EC694572}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1727,12 +1727,6 @@
     <t>Correggere anagrafica paziente</t>
   </si>
   <si>
-    <t>76fe52d2ec57f95d</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.7755b73f171852c</t>
-  </si>
-  <si>
     <t>UNKNOWN_WORKFLOW_ID</t>
   </si>
   <si>
@@ -1784,10 +1778,16 @@
     <t>2025-04-08T11:31:54.673Z</t>
   </si>
   <si>
-    <t>2025-04-08T12:45:08.007Z</t>
-  </si>
-  <si>
     <t xml:space="preserve">7599619418747600 </t>
+  </si>
+  <si>
+    <t>2025-05-09T17:55:55.273Z</t>
+  </si>
+  <si>
+    <t>e5ae4fedb925ec1913ef57339f640284</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.23c41309a8842ba</t>
   </si>
 </sst>
 </file>
@@ -2384,6 +2384,9 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2405,9 +2408,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2705,7 +2705,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A13"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -2784,7 +2784,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B996"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -3855,10 +3855,10 @@
   <dimension ref="A1:W756"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="E15" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="F131" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="H15" sqref="H15"/>
+      <selection pane="bottomRight" activeCell="I170" sqref="I170"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3902,14 +3902,14 @@
       <c r="W1" s="9"/>
     </row>
     <row r="2" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="47" t="s">
+      <c r="A2" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="48"/>
-      <c r="C2" s="49" t="s">
+      <c r="B2" s="49"/>
+      <c r="C2" s="50" t="s">
         <v>434</v>
       </c>
-      <c r="D2" s="48"/>
+      <c r="D2" s="49"/>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
       <c r="H2" s="6"/>
@@ -3930,14 +3930,14 @@
       <c r="W2" s="9"/>
     </row>
     <row r="3" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="50" t="s">
+      <c r="A3" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="51"/>
-      <c r="C3" s="56" t="s">
+      <c r="B3" s="52"/>
+      <c r="C3" s="57" t="s">
         <v>435</v>
       </c>
-      <c r="D3" s="48"/>
+      <c r="D3" s="49"/>
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
@@ -3958,12 +3958,12 @@
       <c r="W3" s="9"/>
     </row>
     <row r="4" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="52"/>
-      <c r="B4" s="53"/>
-      <c r="C4" s="56" t="s">
+      <c r="A4" s="53"/>
+      <c r="B4" s="54"/>
+      <c r="C4" s="57" t="s">
         <v>436</v>
       </c>
-      <c r="D4" s="48"/>
+      <c r="D4" s="49"/>
       <c r="E4" s="4"/>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
@@ -3985,12 +3985,12 @@
       <c r="W4" s="9"/>
     </row>
     <row r="5" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="54"/>
-      <c r="B5" s="55"/>
-      <c r="C5" s="56" t="s">
+      <c r="A5" s="55"/>
+      <c r="B5" s="56"/>
+      <c r="C5" s="57" t="s">
         <v>437</v>
       </c>
-      <c r="D5" s="48"/>
+      <c r="D5" s="49"/>
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
@@ -4011,8 +4011,8 @@
       <c r="W5" s="9"/>
     </row>
     <row r="6" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="45"/>
-      <c r="B6" s="46"/>
+      <c r="A6" s="46"/>
+      <c r="B6" s="47"/>
       <c r="C6" s="10"/>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
@@ -4352,13 +4352,13 @@
         <v>45755</v>
       </c>
       <c r="G15" s="33" t="s">
-        <v>457</v>
-      </c>
-      <c r="H15" s="57" t="s">
-        <v>462</v>
+        <v>455</v>
+      </c>
+      <c r="H15" s="45" t="s">
+        <v>459</v>
       </c>
       <c r="I15" s="39" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="J15" s="29" t="s">
         <v>66</v>
@@ -4372,7 +4372,7 @@
         <v>66</v>
       </c>
       <c r="O15" s="29" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="P15" s="29" t="s">
         <v>66</v>
@@ -4384,7 +4384,7 @@
         <v>66</v>
       </c>
       <c r="S15" s="29" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="T15" s="29"/>
       <c r="U15" s="34"/>
@@ -4672,13 +4672,13 @@
         <v>45755</v>
       </c>
       <c r="G23" s="33" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="H23" s="33" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="I23" s="39" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="J23" s="29" t="s">
         <v>66</v>
@@ -4692,7 +4692,7 @@
         <v>66</v>
       </c>
       <c r="O23" s="29" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="P23" s="29" t="s">
         <v>66</v>
@@ -4704,7 +4704,7 @@
         <v>66</v>
       </c>
       <c r="S23" s="29" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="T23" s="29"/>
       <c r="U23" s="34"/>
@@ -5000,7 +5000,7 @@
         <v>45755</v>
       </c>
       <c r="G31" s="33" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="H31" s="33"/>
       <c r="I31" s="39"/>
@@ -5016,7 +5016,7 @@
         <v>66</v>
       </c>
       <c r="O31" s="29" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="P31" s="29" t="s">
         <v>66</v>
@@ -5028,7 +5028,7 @@
         <v>66</v>
       </c>
       <c r="S31" s="29" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="T31" s="29"/>
       <c r="U31" s="34" t="s">
@@ -5069,7 +5069,7 @@
       <c r="Q32" s="29"/>
       <c r="R32" s="29"/>
       <c r="S32" s="29" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="T32" s="29"/>
       <c r="U32" s="34" t="s">
@@ -5110,7 +5110,7 @@
       <c r="Q33" s="29"/>
       <c r="R33" s="29"/>
       <c r="S33" s="29" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="T33" s="29"/>
       <c r="U33" s="34" t="s">
@@ -5151,7 +5151,7 @@
       <c r="Q34" s="29"/>
       <c r="R34" s="29"/>
       <c r="S34" s="29" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="T34" s="29"/>
       <c r="U34" s="34" t="s">
@@ -5192,7 +5192,7 @@
       <c r="Q35" s="29"/>
       <c r="R35" s="29"/>
       <c r="S35" s="29" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="T35" s="29"/>
       <c r="U35" s="34"/>
@@ -5231,7 +5231,7 @@
       <c r="Q36" s="29"/>
       <c r="R36" s="29"/>
       <c r="S36" s="29" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="T36" s="29"/>
       <c r="U36" s="34"/>
@@ -8220,7 +8220,7 @@
         <v>45755</v>
       </c>
       <c r="G117" s="33" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="H117" s="33" t="s">
         <v>438</v>
@@ -10262,16 +10262,16 @@
         <v>399</v>
       </c>
       <c r="F170" s="33">
-        <v>45755</v>
+        <v>45786</v>
       </c>
       <c r="G170" s="33" t="s">
+        <v>460</v>
+      </c>
+      <c r="H170" s="33" t="s">
         <v>461</v>
       </c>
-      <c r="H170" s="33" t="s">
-        <v>442</v>
-      </c>
       <c r="I170" s="39" t="s">
-        <v>443</v>
+        <v>462</v>
       </c>
       <c r="J170" s="29" t="s">
         <v>66</v>
@@ -17488,27 +17488,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A92AB09DCDF6014AA0D6826BF29E2C8E" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d4db60622090a1f8a8d506ac1d64a349">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1e76d14e-d0ce-457c-8343-9b55836d9ead" xmlns:ns3="a56712a3-8dfd-4688-917a-22f0cf513b89" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0a3a9ed8bb952a3d76dd1e2fa3d624b9" ns2:_="" ns3:_="">
     <xsd:import namespace="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
@@ -17766,7 +17745,47 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1CE213DB-5082-48B0-B2A5-099EBF944035}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
+    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
@@ -17783,29 +17802,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1CE213DB-5082-48B0-B2A5-099EBF944035}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
-    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>